<commit_message>
An information column is added
</commit_message>
<xml_diff>
--- a/LoRa.xlsx
+++ b/LoRa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Perez\Documents\GitHub\TTN-LoRaWAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33D762B-58BD-406C-B6E8-E20D8E3CEDFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F88411E-CFC2-47D5-8F2D-9FB512F6C495}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,22 +16,34 @@
     <sheet name="GENERAL" sheetId="1" r:id="rId1"/>
     <sheet name="MAPINFO" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERAL!$B$2:$Y$7</definedName>
-  </definedNames>
   <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+  <si>
+    <t>DEVICE</t>
+  </si>
+  <si>
+    <t>METADATA</t>
+  </si>
+  <si>
+    <t>GATEWAY 1</t>
+  </si>
+  <si>
+    <t>GATEWAY 2</t>
+  </si>
+  <si>
+    <t>GATEWAY 3</t>
+  </si>
+  <si>
+    <t>GATEWAY 4</t>
+  </si>
   <si>
     <t>GRUPO</t>
   </si>
   <si>
-    <t>DEVICE</t>
-  </si>
-  <si>
     <t>SERIAL</t>
   </si>
   <si>
@@ -68,12 +80,33 @@
     <t>GW1</t>
   </si>
   <si>
+    <t>TSTAMP1</t>
+  </si>
+  <si>
+    <t>TIME1</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>RSSI1</t>
+  </si>
+  <si>
     <t>SNR1</t>
   </si>
   <si>
     <t>GW2</t>
   </si>
   <si>
+    <t>TSTAMP2</t>
+  </si>
+  <si>
+    <t>TIME2</t>
+  </si>
+  <si>
+    <t>CH2</t>
+  </si>
+  <si>
     <t>RSSI2</t>
   </si>
   <si>
@@ -83,6 +116,15 @@
     <t>GW3</t>
   </si>
   <si>
+    <t>TSTAMP3</t>
+  </si>
+  <si>
+    <t>TIME3</t>
+  </si>
+  <si>
+    <t>CH3</t>
+  </si>
+  <si>
     <t>RSSI3</t>
   </si>
   <si>
@@ -92,64 +134,79 @@
     <t>GW4</t>
   </si>
   <si>
+    <t>TSTAMP4</t>
+  </si>
+  <si>
+    <t>TIME4</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
     <t>RSSI4</t>
   </si>
   <si>
     <t>SNR4</t>
   </si>
   <si>
-    <t>TIME1</t>
-  </si>
-  <si>
-    <t>TSTAMP1</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>RSSI1</t>
-  </si>
-  <si>
-    <t>TSTAMP2</t>
-  </si>
-  <si>
-    <t>TIME2</t>
-  </si>
-  <si>
-    <t>CH2</t>
-  </si>
-  <si>
-    <t>TSTAMP3</t>
-  </si>
-  <si>
-    <t>TIME3</t>
-  </si>
-  <si>
-    <t>CH3</t>
-  </si>
-  <si>
-    <t>METADATA</t>
-  </si>
-  <si>
-    <t>GATEWAY 1</t>
-  </si>
-  <si>
-    <t>GATEWAY 2</t>
-  </si>
-  <si>
-    <t>GATEWAY 3</t>
-  </si>
-  <si>
-    <t>TSTAMP4</t>
-  </si>
-  <si>
-    <t>TIME4</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>GATEWAY 4</t>
+    <t>beacon-encontrack</t>
+  </si>
+  <si>
+    <t>guppy</t>
+  </si>
+  <si>
+    <t>70B3D570500029DA</t>
+  </si>
+  <si>
+    <t>Z4A=</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:58:51.806935466Z</t>
+  </si>
+  <si>
+    <t>LORA</t>
+  </si>
+  <si>
+    <t>SF10BW125</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>eui-7276ff00080d082d</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:58:51.70476Z</t>
+  </si>
+  <si>
+    <t>eui-7276ff00080d08c0</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:58:51.715013Z</t>
+  </si>
+  <si>
+    <t>Z4E=</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:58:59.986586403Z</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:58:59.892157Z</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:58:59.882426Z</t>
+  </si>
+  <si>
+    <t>ZoA=</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:59:06.49086737Z</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:59:06.403533Z</t>
+  </si>
+  <si>
+    <t>2019-08-20T22:59:06.393802Z</t>
   </si>
 </sst>
 </file>
@@ -225,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -251,37 +308,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,224 +664,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G10:G13"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" style="10" customWidth="1"/>
-    <col min="27" max="27" width="10.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10" style="11" customWidth="1"/>
-    <col min="29" max="29" width="6.75" style="11" customWidth="1"/>
-    <col min="30" max="30" width="8.75" style="11" customWidth="1"/>
-    <col min="31" max="31" width="6.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11" style="10"/>
-    <col min="33" max="36" width="11" style="11"/>
-    <col min="37" max="37" width="6.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.75" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:37" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="11"/>
+    </row>
+    <row r="2" spans="1:37" s="5" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="6" t="s">
+      <c r="AE2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="6" t="s">
+      <c r="AF2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="6" t="s">
+      <c r="AG2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="6" t="s">
+      <c r="AH2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="12"/>
     </row>
-    <row r="2" spans="1:37" s="1" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="16">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16">
+        <v>4994</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="16">
+        <v>905.1</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="16">
+        <v>329728000</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="8">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="16">
+        <v>377176084</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="16">
+        <v>6</v>
+      </c>
+      <c r="R3" s="16">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="S3" s="8">
+        <v>11.8</v>
+      </c>
+      <c r="T3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U3">
+        <v>1998916900</v>
+      </c>
+      <c r="V3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W3">
+        <v>6</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E4" s="16">
+        <v>4995</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="16">
+        <v>905.3</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="16">
+        <v>329728000</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="N4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="16">
+        <v>2007094444</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>7</v>
+      </c>
+      <c r="R4" s="16">
+        <v>0</v>
+      </c>
+      <c r="S4" s="8">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="T4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4">
+        <v>385353636</v>
+      </c>
+      <c r="V4" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4">
+        <v>7</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>4996</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="16">
+        <v>904.9</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="16">
+        <v>329728000</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="8">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="16">
+        <v>2013605820</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="16">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>23</v>
+      <c r="R5" s="16">
+        <v>0</v>
+      </c>
+      <c r="S5" s="8">
+        <v>12.2</v>
+      </c>
+      <c r="T5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5">
+        <v>391865012</v>
+      </c>
+      <c r="V5" t="s">
+        <v>61</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>13.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AF1:AK1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="Z1:AE1"/>
-    <mergeCell ref="AF1:AK1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
An example is added
</commit_message>
<xml_diff>
--- a/LoRa.xlsx
+++ b/LoRa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Perez\Documents\GitHub\TTN-LoRaWAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F88411E-CFC2-47D5-8F2D-9FB512F6C495}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF03DAE-AAC0-44A1-8D0F-D79A54750C08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,7 +667,7 @@
   <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
convert payload from base64 to hexadecimal
</commit_message>
<xml_diff>
--- a/LoRa.xlsx
+++ b/LoRa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Perez\Documents\GitHub\TTN-LoRaWAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF03DAE-AAC0-44A1-8D0F-D79A54750C08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE157C7-E6B7-4C15-8F52-C9A288413604}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,15 @@
     <sheet name="GENERAL" sheetId="1" r:id="rId1"/>
     <sheet name="MAPINFO" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERAL!$A$2:$AK$95</definedName>
+  </definedNames>
   <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>DEVICE</t>
   </si>
@@ -147,66 +150,6 @@
   </si>
   <si>
     <t>SNR4</t>
-  </si>
-  <si>
-    <t>beacon-encontrack</t>
-  </si>
-  <si>
-    <t>guppy</t>
-  </si>
-  <si>
-    <t>70B3D570500029DA</t>
-  </si>
-  <si>
-    <t>Z4A=</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:58:51.806935466Z</t>
-  </si>
-  <si>
-    <t>LORA</t>
-  </si>
-  <si>
-    <t>SF10BW125</t>
-  </si>
-  <si>
-    <t>4/5</t>
-  </si>
-  <si>
-    <t>eui-7276ff00080d082d</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:58:51.70476Z</t>
-  </si>
-  <si>
-    <t>eui-7276ff00080d08c0</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:58:51.715013Z</t>
-  </si>
-  <si>
-    <t>Z4E=</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:58:59.986586403Z</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:58:59.892157Z</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:58:59.882426Z</t>
-  </si>
-  <si>
-    <t>ZoA=</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:59:06.49086737Z</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:59:06.403533Z</t>
-  </si>
-  <si>
-    <t>2019-08-20T22:59:06.393802Z</t>
   </si>
 </sst>
 </file>
@@ -323,14 +266,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -344,12 +287,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,79 +610,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.75" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.375" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5" style="8" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.625" style="7" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="11"/>
       <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
       <c r="M1" s="11"/>
       <c r="N1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="U1" s="10"/>
@@ -744,7 +690,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="AA1" s="10"/>
@@ -761,20 +707,20 @@
       <c r="AJ1" s="10"/>
       <c r="AK1" s="11"/>
     </row>
-    <row r="2" spans="1:37" s="5" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:37" s="6" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -798,58 +744,58 @@
       <c r="L2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="20" t="s">
         <v>22</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AB2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AC2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AD2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AE2" s="3" t="s">
@@ -858,16 +804,16 @@
       <c r="AF2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AG2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AI2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>40</v>
       </c>
       <c r="AK2" s="3" t="s">
@@ -875,237 +821,111 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>4994</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="16">
-        <v>905.1</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="16">
-        <v>329728000</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="8">
-        <v>2</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" s="16">
-        <v>377176084</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" s="16">
-        <v>6</v>
-      </c>
-      <c r="R3" s="16">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8">
-        <v>11.8</v>
-      </c>
-      <c r="T3" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3">
-        <v>1998916900</v>
-      </c>
-      <c r="V3" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3">
-        <v>6</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>12.5</v>
-      </c>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16">
-        <v>4995</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="16">
-        <v>905.3</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="16">
-        <v>329728000</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="8">
-        <v>2</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="16">
-        <v>2007094444</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q4" s="16">
-        <v>7</v>
-      </c>
-      <c r="R4" s="16">
-        <v>0</v>
-      </c>
-      <c r="S4" s="8">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="T4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4">
-        <v>385353636</v>
-      </c>
-      <c r="V4" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4">
-        <v>7</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>10.5</v>
-      </c>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="16">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16">
-        <v>4996</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="16">
-        <v>904.9</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="16">
-        <v>329728000</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="8">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" s="16">
-        <v>2013605820</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5" s="16">
-        <v>5</v>
-      </c>
-      <c r="R5" s="16">
-        <v>0</v>
-      </c>
-      <c r="S5" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="T5" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5">
-        <v>391865012</v>
-      </c>
-      <c r="V5" t="s">
-        <v>61</v>
-      </c>
-      <c r="W5">
-        <v>5</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>13.5</v>
-      </c>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AK95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="6">
     <mergeCell ref="AF1:AK1"/>
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
The way the data is processed is changed, because the fields vary depending on the configuration of the gateways.
</commit_message>
<xml_diff>
--- a/LoRa.xlsx
+++ b/LoRa.xlsx
@@ -8,45 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Perez\Documents\GitHub\TTN-LoRaWAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE157C7-E6B7-4C15-8F52-C9A288413604}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71A2698-8E04-4849-BD39-1A3E82BB6D87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="1" r:id="rId1"/>
-    <sheet name="MAPINFO" sheetId="2" r:id="rId2"/>
+    <sheet name="OYSTER" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERAL!$A$2:$AK$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERAL!$A$2:$AS$95</definedName>
   </definedNames>
   <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>METADATA</t>
+  </si>
+  <si>
+    <t>GATEWAY 1</t>
+  </si>
+  <si>
+    <t>GATEWAY 2</t>
+  </si>
+  <si>
+    <t>GATEWAY 3</t>
+  </si>
+  <si>
+    <t>GATEWAY 4</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
   <si>
     <t>DEVICE</t>
   </si>
   <si>
-    <t>METADATA</t>
-  </si>
-  <si>
-    <t>GATEWAY 1</t>
-  </si>
-  <si>
-    <t>GATEWAY 2</t>
-  </si>
-  <si>
-    <t>GATEWAY 3</t>
-  </si>
-  <si>
-    <t>GATEWAY 4</t>
-  </si>
-  <si>
-    <t>GRUPO</t>
-  </si>
-  <si>
     <t>SERIAL</t>
   </si>
   <si>
@@ -98,6 +101,12 @@
     <t>SNR1</t>
   </si>
   <si>
+    <t>LAT1</t>
+  </si>
+  <si>
+    <t>LON1</t>
+  </si>
+  <si>
     <t>GW2</t>
   </si>
   <si>
@@ -116,6 +125,12 @@
     <t>SNR2</t>
   </si>
   <si>
+    <t>LAT2</t>
+  </si>
+  <si>
+    <t>LON2</t>
+  </si>
+  <si>
     <t>GW3</t>
   </si>
   <si>
@@ -134,6 +149,12 @@
     <t>SNR3</t>
   </si>
   <si>
+    <t>LAT3</t>
+  </si>
+  <si>
+    <t>LON3</t>
+  </si>
+  <si>
     <t>GW4</t>
   </si>
   <si>
@@ -150,6 +171,54 @@
   </si>
   <si>
     <t>SNR4</t>
+  </si>
+  <si>
+    <t>LAT4</t>
+  </si>
+  <si>
+    <t>LON4</t>
+  </si>
+  <si>
+    <t>beacons</t>
+  </si>
+  <si>
+    <t>oyster</t>
+  </si>
+  <si>
+    <t>70B3D5705000383F</t>
+  </si>
+  <si>
+    <t>000000000000000003009c</t>
+  </si>
+  <si>
+    <t>2019-08-21T23:06:09.711393186Z</t>
+  </si>
+  <si>
+    <t>LORA</t>
+  </si>
+  <si>
+    <t>SF10BW125</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>viviteclorawan</t>
+  </si>
+  <si>
+    <t>2019-08-21T23:06:09Z</t>
+  </si>
+  <si>
+    <t>eui-7276ff00080d08c0</t>
+  </si>
+  <si>
+    <t>2019-08-21T23:06:09.654598Z</t>
+  </si>
+  <si>
+    <t>eui-7276ff00080d082d</t>
+  </si>
+  <si>
+    <t>2019-08-21T23:06:09.634067Z</t>
   </si>
 </sst>
 </file>
@@ -266,13 +335,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -290,12 +362,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,329 +676,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.375" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.75" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.875" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.625" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="10" customWidth="1"/>
+    <col min="10" max="10" width="11.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.25" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.25" style="10" customWidth="1"/>
+    <col min="20" max="20" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8" style="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8" style="10" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.25" style="10" customWidth="1"/>
+    <col min="44" max="44" width="8.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="13" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="9" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="14" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="14" t="s">
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="9" t="s">
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="11"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="14"/>
     </row>
-    <row r="2" spans="1:37" s="6" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:45" s="9" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3">
+        <v>904.1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3">
+        <v>370688000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3">
+        <v>3039659980</v>
+      </c>
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>-115</v>
+      </c>
+      <c r="S3">
+        <v>-8</v>
+      </c>
+      <c r="T3">
+        <v>20.584993000000001</v>
+      </c>
+      <c r="U3">
+        <v>-100.37957</v>
+      </c>
+      <c r="V3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W3">
+        <v>718772748</v>
+      </c>
+      <c r="X3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
-      <c r="Y15"/>
+      <c r="AA3">
+        <v>11.8</v>
+      </c>
+      <c r="AB3">
+        <v>20.576433000000002</v>
+      </c>
+      <c r="AC3">
+        <v>-100.36094</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE3">
+        <v>2494212356</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>12.8</v>
+      </c>
+      <c r="AJ3">
+        <v>20.574771999999999</v>
+      </c>
+      <c r="AK3">
+        <v>-100.35972</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AK95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:AS95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="6">
-    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AS1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:M1"/>
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AD1:AK1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -943,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>